<commit_message>
save data done + era data updated
</commit_message>
<xml_diff>
--- a/2021_era_data.xlsx
+++ b/2021_era_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C910"/>
+  <dimension ref="A1:C927"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12268,6 +12268,227 @@
         <v>6.26</v>
       </c>
     </row>
+    <row r="911">
+      <c r="A911" s="1" t="n">
+        <v>909</v>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>ángel perdomo</t>
+        </is>
+      </c>
+      <c r="C911" t="n">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" s="1" t="n">
+        <v>910</v>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>brent honeywell</t>
+        </is>
+      </c>
+      <c r="C912" t="n">
+        <v>8.31</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" s="1" t="n">
+        <v>911</v>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>carl edwards</t>
+        </is>
+      </c>
+      <c r="C913" t="n">
+        <v>11.12</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="1" t="n">
+        <v>912</v>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>dan camarena</t>
+        </is>
+      </c>
+      <c r="C914" t="n">
+        <v>9.640000000000001</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" s="1" t="n">
+        <v>913</v>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>daniel lynch</t>
+        </is>
+      </c>
+      <c r="C915" t="n">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="1" t="n">
+        <v>914</v>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>duane underwood</t>
+        </is>
+      </c>
+      <c r="C916" t="n">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" s="1" t="n">
+        <v>915</v>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>j.b. bukauskas</t>
+        </is>
+      </c>
+      <c r="C917" t="n">
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" s="1" t="n">
+        <v>916</v>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>j.t. chargois</t>
+        </is>
+      </c>
+      <c r="C918" t="n">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="1" t="n">
+        <v>917</v>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>jaime barría</t>
+        </is>
+      </c>
+      <c r="C919" t="n">
+        <v>4.61</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="1" t="n">
+        <v>918</v>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>julio teherán</t>
+        </is>
+      </c>
+      <c r="C920" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="1" t="n">
+        <v>919</v>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>lance mccullers</t>
+        </is>
+      </c>
+      <c r="C921" t="n">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" s="1" t="n">
+        <v>920</v>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>matt boyd</t>
+        </is>
+      </c>
+      <c r="C922" t="n">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" s="1" t="n">
+        <v>921</v>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>mike king</t>
+        </is>
+      </c>
+      <c r="C923" t="n">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" s="1" t="n">
+        <v>922</v>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>mike wright</t>
+        </is>
+      </c>
+      <c r="C924" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" s="1" t="n">
+        <v>923</v>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>néstor cortés</t>
+        </is>
+      </c>
+      <c r="C925" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" s="1" t="n">
+        <v>924</v>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>travis lakins</t>
+        </is>
+      </c>
+      <c r="C926" t="n">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" s="1" t="n">
+        <v>925</v>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>vladimir gutiérrez</t>
+        </is>
+      </c>
+      <c r="C927" t="n">
+        <v>4.74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>